<commit_message>
Login & Sign Up
</commit_message>
<xml_diff>
--- a/TEMPS/database-ecommerce.xlsx
+++ b/TEMPS/database-ecommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Django\mysite\TEMPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61748E1-1697-4044-8CBF-79D27EEB04F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DE2E15-F0FC-4926-8A08-B1351F319C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{95E6102E-BFE5-48CA-B125-283D6CE05FC7}"/>
   </bookViews>
@@ -214,12 +214,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Orders</t>
-  </si>
-  <si>
-    <t>Oders_Products</t>
-  </si>
-  <si>
     <t>Setting</t>
   </si>
   <si>
@@ -257,6 +251,12 @@
   </si>
   <si>
     <t>ShopCart</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Oders_Product</t>
   </si>
 </sst>
 </file>
@@ -975,6 +975,70 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>923924</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Ok: Bükülü 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1AA3D0-2BCD-4ACB-9DD3-772CF926AC38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="8924924" y="3719513"/>
+          <a:ext cx="1185863" cy="1119187"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="tr-TR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1278,7 +1342,7 @@
   <dimension ref="B1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,12 +1371,12 @@
   <sheetData>
     <row r="1" spans="2:20" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J1" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
@@ -1332,15 +1396,15 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="21" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="21" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="4" t="s">
@@ -1406,7 +1470,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="10" t="s">
@@ -1414,7 +1478,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="16" t="s">
@@ -1463,7 +1527,7 @@
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="5" t="s">
@@ -1484,7 +1548,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="10" t="s">
@@ -1504,7 +1568,7 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="5" t="s">
@@ -1572,7 +1636,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1582,7 +1646,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="16" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="5" t="s">
@@ -1646,7 +1710,7 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3" t="s">
@@ -1687,7 +1751,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1757,7 +1821,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="16" t="s">
@@ -1780,7 +1844,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1866,7 +1930,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -1944,7 +2008,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O20" s="2"/>
       <c r="Q20" s="2"/>
@@ -1969,7 +2033,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O21" s="2"/>
       <c r="Q21" s="2"/>

</xml_diff>

<commit_message>
User panel, Update User inf
</commit_message>
<xml_diff>
--- a/TEMPS/database-ecommerce.xlsx
+++ b/TEMPS/database-ecommerce.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Django\mysite\TEMPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75C2CB9-DF80-492C-B908-1CC690CDEAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89EE002-49F3-4D94-A2DE-FF2142387D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{95E6102E-BFE5-48CA-B125-283D6CE05FC7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
   <si>
     <t>user</t>
   </si>
@@ -257,13 +257,37 @@
   </si>
   <si>
     <t>Oder_Product</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>menu_id</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>content_id</t>
+  </si>
+  <si>
+    <t>cimages</t>
+  </si>
+  <si>
+    <t>Content Managament System</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>(menu,haber,duyuru)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +326,15 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -370,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -404,11 +437,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,6 +569,22 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A06BE9-8163-4315-8404-44365A89419E}">
-  <dimension ref="B1:T25"/>
+  <dimension ref="B1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +2081,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
@@ -1950,7 +2092,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="22" t="s">
         <v>29</v>
       </c>
       <c r="K18" s="2"/>
@@ -1974,12 +2116,13 @@
         <v>20</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="16" t="s">
@@ -1991,7 +2134,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
         <v>19</v>
       </c>
@@ -1999,12 +2142,19 @@
         <v>20</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" s="28"/>
+      <c r="J20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" s="29"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="16" t="s">
@@ -2024,12 +2174,19 @@
         <v>20</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="28"/>
+      <c r="J21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="29"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="16" t="s">
@@ -2047,12 +2204,19 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="28"/>
+      <c r="J22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="29"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="O22" s="2"/>
@@ -2067,12 +2231,19 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="29"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="O23" s="2"/>
@@ -2085,10 +2256,122 @@
       <c r="B24" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="31"/>
+      <c r="J24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="32"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E25" s="30"/>
+      <c r="F25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="31"/>
+      <c r="H25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="32"/>
       <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E26" s="30"/>
+      <c r="F26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="31"/>
+      <c r="H26" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="32"/>
+    </row>
+    <row r="27" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E27" s="30"/>
+      <c r="F27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="31"/>
+      <c r="H27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32"/>
+    </row>
+    <row r="28" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="32"/>
+    </row>
+    <row r="29" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="32"/>
+    </row>
+    <row r="30" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="32"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="32"/>
+    </row>
+    <row r="32" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E32" s="30"/>
+      <c r="F32" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="32"/>
+    </row>
+    <row r="33" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Variants & Attributes Size Color
</commit_message>
<xml_diff>
--- a/TEMPS/database-ecommerce.xlsx
+++ b/TEMPS/database-ecommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Django\mysite\TEMPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89EE002-49F3-4D94-A2DE-FF2142387D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EC7679-F715-4FF3-A240-847A7695C214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{95E6102E-BFE5-48CA-B125-283D6CE05FC7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
   <si>
     <t>user</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>(menu,haber,duyuru)</t>
+  </si>
+  <si>
+    <t>variants</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>var</t>
   </si>
 </sst>
 </file>
@@ -1181,6 +1190,59 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Düz Ok Bağlayıcısı 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7812BBF5-31B5-4D19-A715-1F51F3161FF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4533900" y="5219700"/>
+          <a:ext cx="428625" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1481,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A06BE9-8163-4315-8404-44365A89419E}">
-  <dimension ref="B1:T33"/>
+  <dimension ref="B1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,14 +1571,17 @@
     <col min="18" max="18" width="13.42578125" customWidth="1"/>
     <col min="19" max="19" width="4" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J1" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
@@ -1556,8 +1621,14 @@
       <c r="T2" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1597,8 +1668,11 @@
       <c r="T3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V3" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1638,8 +1712,11 @@
       <c r="T4" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -1679,8 +1756,11 @@
       <c r="T5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V5" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1720,8 +1800,9 @@
       <c r="T6" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
@@ -1759,8 +1840,9 @@
       <c r="T7" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1798,8 +1880,9 @@
       <c r="T8" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1921,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1875,7 +1958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +1995,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1945,7 +2028,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1974,7 +2057,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2003,7 +2086,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
@@ -2029,7 +2112,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2263,7 @@
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="5" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="5" t="s">
@@ -2210,7 +2293,7 @@
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="5" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="I22" s="28"/>
       <c r="J22" s="5" t="s">
@@ -2237,7 +2320,7 @@
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="5" t="s">
@@ -2257,10 +2340,12 @@
         <v>29</v>
       </c>
       <c r="E24" s="30"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="G24" s="31"/>
       <c r="H24" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="5" t="s">
@@ -2276,7 +2361,7 @@
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="5" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -2289,8 +2374,8 @@
         <v>28</v>
       </c>
       <c r="G26" s="31"/>
-      <c r="H26" s="37" t="s">
-        <v>81</v>
+      <c r="H26" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="I26" s="31" t="s">
         <v>82</v>
@@ -2304,8 +2389,8 @@
         <v>29</v>
       </c>
       <c r="G27" s="31"/>
-      <c r="H27" s="5" t="s">
-        <v>23</v>
+      <c r="H27" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -2316,7 +2401,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
       <c r="H28" s="5" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -2327,7 +2412,7 @@
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
       <c r="H29" s="5" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -2338,17 +2423,19 @@
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
       <c r="H30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
       <c r="K30" s="32"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E31" s="30"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
+      <c r="H31" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
       <c r="K31" s="32"/>

</xml_diff>